<commit_message>
add variance sheet to workbook
</commit_message>
<xml_diff>
--- a/files/Business expense budget.xlsx
+++ b/files/Business expense budget.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD3DFCA-9C52-6D4A-AF25-B7C8CA312861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86440985-1F52-0640-AEB2-BE9EE95A0FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="756" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="756" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="6" r:id="rId1"/>
     <sheet name="PLANNED EXPENSES" sheetId="2" r:id="rId2"/>
     <sheet name="Forecast Expenses Database" sheetId="9" r:id="rId3"/>
     <sheet name="Actuals Expenses Database" sheetId="7" r:id="rId4"/>
-    <sheet name="ACTUAL EXPENSES" sheetId="3" r:id="rId5"/>
-    <sheet name="EXPENSE VARIANCES" sheetId="4" r:id="rId6"/>
-    <sheet name="EXPENSE ANALYSIS" sheetId="5" r:id="rId7"/>
+    <sheet name="Actuals vs Forecast" sheetId="11" r:id="rId5"/>
+    <sheet name="ACTUAL EXPENSES" sheetId="3" r:id="rId6"/>
+    <sheet name="EXPENSE VARIANCES" sheetId="4" r:id="rId7"/>
+    <sheet name="EXPENSE ANALYSIS" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="worksheet_title">'PLANNED EXPENSES'!$O$2</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="69">
   <si>
     <t>Jan</t>
   </si>
@@ -12590,8 +12591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A97BD2-4449-5546-B60F-5442C2C9CEF7}">
   <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="D209" sqref="D209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -15599,8 +15600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED331B49-F4B1-6743-8B96-82C9B897B046}">
   <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D209" sqref="D209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -18605,6 +18606,3159 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84536B2D-73D3-F549-9277-6D6C9E4CF2BB}">
+  <dimension ref="A1:D209"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="O103" sqref="O103"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <f>+'Actuals Expenses Database'!D2-'Forecast Expenses Database'!D2</f>
+        <v>-175.61575140451896</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20">
+        <f>+'Actuals Expenses Database'!D3-'Forecast Expenses Database'!D3</f>
+        <v>-61.973751419209293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="20">
+        <f>+'Actuals Expenses Database'!D4-'Forecast Expenses Database'!D4</f>
+        <v>35.009233026139555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="20">
+        <f>+'Actuals Expenses Database'!D5-'Forecast Expenses Database'!D5</f>
+        <v>-36.380207031659666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="20">
+        <f>+'Actuals Expenses Database'!D6-'Forecast Expenses Database'!D6</f>
+        <v>-236.64682753215311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="20">
+        <f>+'Actuals Expenses Database'!D7-'Forecast Expenses Database'!D7</f>
+        <v>-259.6416087335092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <f>+'Actuals Expenses Database'!D8-'Forecast Expenses Database'!D8</f>
+        <v>-257.68888753905776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="20">
+        <f>+'Actuals Expenses Database'!D9-'Forecast Expenses Database'!D9</f>
+        <v>8.2490632369590458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="20">
+        <f>+'Actuals Expenses Database'!D10-'Forecast Expenses Database'!D10</f>
+        <v>122.09847113938304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="20">
+        <f>+'Actuals Expenses Database'!D11-'Forecast Expenses Database'!D11</f>
+        <v>130.79297468854929</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="20">
+        <f>+'Actuals Expenses Database'!D12-'Forecast Expenses Database'!D12</f>
+        <v>180.94080556448898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="20">
+        <f>+'Actuals Expenses Database'!D13-'Forecast Expenses Database'!D13</f>
+        <v>-16.047957066082745</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="20">
+        <f>+'Actuals Expenses Database'!D14-'Forecast Expenses Database'!D14</f>
+        <v>-566.9044430705253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="20">
+        <f>+'Actuals Expenses Database'!D15-'Forecast Expenses Database'!D15</f>
+        <v>-460.89278134600318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
+        <f>+'Actuals Expenses Database'!D16-'Forecast Expenses Database'!D16</f>
+        <v>195.18682512846863</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="20">
+        <f>+'Actuals Expenses Database'!D17-'Forecast Expenses Database'!D17</f>
+        <v>130.06522491096985</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="20">
+        <f>+'Actuals Expenses Database'!D18-'Forecast Expenses Database'!D18</f>
+        <v>86.034619431367901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="20">
+        <f>+'Actuals Expenses Database'!D19-'Forecast Expenses Database'!D19</f>
+        <v>-112.35679605115365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="20">
+        <f>+'Actuals Expenses Database'!D20-'Forecast Expenses Database'!D20</f>
+        <v>-130.09232193214848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="20">
+        <f>+'Actuals Expenses Database'!D21-'Forecast Expenses Database'!D21</f>
+        <v>137.40625147657192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="20">
+        <f>+'Actuals Expenses Database'!D22-'Forecast Expenses Database'!D22</f>
+        <v>-11.567644152546563</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="20">
+        <f>+'Actuals Expenses Database'!D23-'Forecast Expenses Database'!D23</f>
+        <v>312.07934047389426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="20">
+        <f>+'Actuals Expenses Database'!D24-'Forecast Expenses Database'!D24</f>
+        <v>-123.51479146716156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="20">
+        <f>+'Actuals Expenses Database'!D25-'Forecast Expenses Database'!D25</f>
+        <v>-274.50875612922755</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="20">
+        <f>+'Actuals Expenses Database'!D26-'Forecast Expenses Database'!D26</f>
+        <v>100.61711529588865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="20">
+        <f>+'Actuals Expenses Database'!D27-'Forecast Expenses Database'!D27</f>
+        <v>-151.54371436109068</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="20">
+        <f>+'Actuals Expenses Database'!D28-'Forecast Expenses Database'!D28</f>
+        <v>-636.50853275052214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="20">
+        <f>+'Actuals Expenses Database'!D29-'Forecast Expenses Database'!D29</f>
+        <v>133.21307370925206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="20">
+        <f>+'Actuals Expenses Database'!D30-'Forecast Expenses Database'!D30</f>
+        <v>165.0744579371094</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="20">
+        <f>+'Actuals Expenses Database'!D31-'Forecast Expenses Database'!D31</f>
+        <v>49.654412399715511</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="20">
+        <f>+'Actuals Expenses Database'!D32-'Forecast Expenses Database'!D32</f>
+        <v>-349.0036235833104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="20">
+        <f>+'Actuals Expenses Database'!D33-'Forecast Expenses Database'!D33</f>
+        <v>-389.7339306656504</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="20">
+        <f>+'Actuals Expenses Database'!D34-'Forecast Expenses Database'!D34</f>
+        <v>-120.28263606248947</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="20">
+        <f>+'Actuals Expenses Database'!D35-'Forecast Expenses Database'!D35</f>
+        <v>-3.3185809155838797</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="20">
+        <f>+'Actuals Expenses Database'!D36-'Forecast Expenses Database'!D36</f>
+        <v>434.1778116132773</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="20">
+        <f>+'Actuals Expenses Database'!D37-'Forecast Expenses Database'!D37</f>
+        <v>7.2781832213804591</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="20">
+        <f>+'Actuals Expenses Database'!D38-'Forecast Expenses Database'!D38</f>
+        <v>-93.567950564742205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="20">
+        <f>+'Actuals Expenses Database'!D39-'Forecast Expenses Database'!D39</f>
+        <v>84.569158229802269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="20">
+        <f>+'Actuals Expenses Database'!D40-'Forecast Expenses Database'!D40</f>
+        <v>-718.44815743179061</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="20">
+        <f>+'Actuals Expenses Database'!D41-'Forecast Expenses Database'!D41</f>
+        <v>259.38667666388938</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="20">
+        <f>+'Actuals Expenses Database'!D42-'Forecast Expenses Database'!D42</f>
+        <v>81.891824252283186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="20">
+        <f>+'Actuals Expenses Database'!D43-'Forecast Expenses Database'!D43</f>
+        <v>353.57609164751011</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="20">
+        <f>+'Actuals Expenses Database'!D44-'Forecast Expenses Database'!D44</f>
+        <v>-347.55712091463465</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="20">
+        <f>+'Actuals Expenses Database'!D45-'Forecast Expenses Database'!D45</f>
+        <v>-145.72449053300807</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="20">
+        <f>+'Actuals Expenses Database'!D46-'Forecast Expenses Database'!D46</f>
+        <v>-131.2961608459118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="20">
+        <f>+'Actuals Expenses Database'!D47-'Forecast Expenses Database'!D47</f>
+        <v>61.586654805514627</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="20">
+        <f>+'Actuals Expenses Database'!D48-'Forecast Expenses Database'!D48</f>
+        <v>-89.272444095720857</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="20">
+        <f>+'Actuals Expenses Database'!D49-'Forecast Expenses Database'!D49</f>
+        <v>48.597046997658254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="20">
+        <f>+'Actuals Expenses Database'!D50-'Forecast Expenses Database'!D50</f>
+        <v>184.16184482483368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="20">
+        <f>+'Actuals Expenses Database'!D51-'Forecast Expenses Database'!D51</f>
+        <v>68.955421072108948</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="20">
+        <f>+'Actuals Expenses Database'!D52-'Forecast Expenses Database'!D52</f>
+        <v>338.36323291375447</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="20">
+        <f>+'Actuals Expenses Database'!D53-'Forecast Expenses Database'!D53</f>
+        <v>682.66857678827364</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="20">
+        <f>+'Actuals Expenses Database'!D54-'Forecast Expenses Database'!D54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="20">
+        <f>+'Actuals Expenses Database'!D55-'Forecast Expenses Database'!D55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="20">
+        <f>+'Actuals Expenses Database'!D56-'Forecast Expenses Database'!D56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="20">
+        <f>+'Actuals Expenses Database'!D57-'Forecast Expenses Database'!D57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="20">
+        <f>+'Actuals Expenses Database'!D58-'Forecast Expenses Database'!D58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="20">
+        <f>+'Actuals Expenses Database'!D59-'Forecast Expenses Database'!D59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="20">
+        <f>+'Actuals Expenses Database'!D60-'Forecast Expenses Database'!D60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="20">
+        <f>+'Actuals Expenses Database'!D61-'Forecast Expenses Database'!D61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="20">
+        <f>+'Actuals Expenses Database'!D62-'Forecast Expenses Database'!D62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="20">
+        <f>+'Actuals Expenses Database'!D63-'Forecast Expenses Database'!D63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="20">
+        <f>+'Actuals Expenses Database'!D64-'Forecast Expenses Database'!D64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="20">
+        <f>+'Actuals Expenses Database'!D65-'Forecast Expenses Database'!D65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="20">
+        <f>+'Actuals Expenses Database'!D66-'Forecast Expenses Database'!D66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="20">
+        <f>+'Actuals Expenses Database'!D67-'Forecast Expenses Database'!D67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="20">
+        <f>+'Actuals Expenses Database'!D68-'Forecast Expenses Database'!D68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="20">
+        <f>+'Actuals Expenses Database'!D69-'Forecast Expenses Database'!D69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="20">
+        <f>+'Actuals Expenses Database'!D70-'Forecast Expenses Database'!D70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="20">
+        <f>+'Actuals Expenses Database'!D71-'Forecast Expenses Database'!D71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="20">
+        <f>+'Actuals Expenses Database'!D72-'Forecast Expenses Database'!D72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="20">
+        <f>+'Actuals Expenses Database'!D73-'Forecast Expenses Database'!D73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="20">
+        <f>+'Actuals Expenses Database'!D74-'Forecast Expenses Database'!D74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="20">
+        <f>+'Actuals Expenses Database'!D75-'Forecast Expenses Database'!D75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="20">
+        <f>+'Actuals Expenses Database'!D76-'Forecast Expenses Database'!D76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="20">
+        <f>+'Actuals Expenses Database'!D77-'Forecast Expenses Database'!D77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="20">
+        <f>+'Actuals Expenses Database'!D78-'Forecast Expenses Database'!D78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="20">
+        <f>+'Actuals Expenses Database'!D79-'Forecast Expenses Database'!D79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="20">
+        <f>+'Actuals Expenses Database'!D80-'Forecast Expenses Database'!D80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="20">
+        <f>+'Actuals Expenses Database'!D81-'Forecast Expenses Database'!D81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="20">
+        <f>+'Actuals Expenses Database'!D82-'Forecast Expenses Database'!D82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="20">
+        <f>+'Actuals Expenses Database'!D83-'Forecast Expenses Database'!D83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="20">
+        <f>+'Actuals Expenses Database'!D84-'Forecast Expenses Database'!D84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="20">
+        <f>+'Actuals Expenses Database'!D85-'Forecast Expenses Database'!D85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="20">
+        <f>+'Actuals Expenses Database'!D86-'Forecast Expenses Database'!D86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="20">
+        <f>+'Actuals Expenses Database'!D87-'Forecast Expenses Database'!D87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="20">
+        <f>+'Actuals Expenses Database'!D88-'Forecast Expenses Database'!D88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="20">
+        <f>+'Actuals Expenses Database'!D89-'Forecast Expenses Database'!D89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="20">
+        <f>+'Actuals Expenses Database'!D90-'Forecast Expenses Database'!D90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="20">
+        <f>+'Actuals Expenses Database'!D91-'Forecast Expenses Database'!D91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="20">
+        <f>+'Actuals Expenses Database'!D92-'Forecast Expenses Database'!D92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="20">
+        <f>+'Actuals Expenses Database'!D93-'Forecast Expenses Database'!D93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" s="20">
+        <f>+'Actuals Expenses Database'!D94-'Forecast Expenses Database'!D94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="20">
+        <f>+'Actuals Expenses Database'!D95-'Forecast Expenses Database'!D95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="20">
+        <f>+'Actuals Expenses Database'!D96-'Forecast Expenses Database'!D96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="20">
+        <f>+'Actuals Expenses Database'!D97-'Forecast Expenses Database'!D97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="20">
+        <f>+'Actuals Expenses Database'!D98-'Forecast Expenses Database'!D98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="20">
+        <f>+'Actuals Expenses Database'!D99-'Forecast Expenses Database'!D99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="20">
+        <f>+'Actuals Expenses Database'!D100-'Forecast Expenses Database'!D100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="20">
+        <f>+'Actuals Expenses Database'!D101-'Forecast Expenses Database'!D101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="20">
+        <f>+'Actuals Expenses Database'!D102-'Forecast Expenses Database'!D102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" s="20">
+        <f>+'Actuals Expenses Database'!D103-'Forecast Expenses Database'!D103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="20">
+        <f>+'Actuals Expenses Database'!D104-'Forecast Expenses Database'!D104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" s="20">
+        <f>+'Actuals Expenses Database'!D105-'Forecast Expenses Database'!D105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="20">
+        <f>+'Actuals Expenses Database'!D106-'Forecast Expenses Database'!D106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107" s="20">
+        <f>+'Actuals Expenses Database'!D107-'Forecast Expenses Database'!D107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="20">
+        <f>+'Actuals Expenses Database'!D108-'Forecast Expenses Database'!D108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="20">
+        <f>+'Actuals Expenses Database'!D109-'Forecast Expenses Database'!D109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="20">
+        <f>+'Actuals Expenses Database'!D110-'Forecast Expenses Database'!D110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="20">
+        <f>+'Actuals Expenses Database'!D111-'Forecast Expenses Database'!D111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B112" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="20">
+        <f>+'Actuals Expenses Database'!D112-'Forecast Expenses Database'!D112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="20">
+        <f>+'Actuals Expenses Database'!D113-'Forecast Expenses Database'!D113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" s="20">
+        <f>+'Actuals Expenses Database'!D114-'Forecast Expenses Database'!D114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="20">
+        <f>+'Actuals Expenses Database'!D115-'Forecast Expenses Database'!D115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" s="20">
+        <f>+'Actuals Expenses Database'!D116-'Forecast Expenses Database'!D116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="20">
+        <f>+'Actuals Expenses Database'!D117-'Forecast Expenses Database'!D117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C118" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="20">
+        <f>+'Actuals Expenses Database'!D118-'Forecast Expenses Database'!D118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C119" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="20">
+        <f>+'Actuals Expenses Database'!D119-'Forecast Expenses Database'!D119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B120" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120" s="20">
+        <f>+'Actuals Expenses Database'!D120-'Forecast Expenses Database'!D120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B121" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" s="20">
+        <f>+'Actuals Expenses Database'!D121-'Forecast Expenses Database'!D121</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D122" s="20">
+        <f>+'Actuals Expenses Database'!D122-'Forecast Expenses Database'!D122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B123" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C123" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D123" s="20">
+        <f>+'Actuals Expenses Database'!D123-'Forecast Expenses Database'!D123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B124" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C124" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="20">
+        <f>+'Actuals Expenses Database'!D124-'Forecast Expenses Database'!D124</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="20">
+        <f>+'Actuals Expenses Database'!D125-'Forecast Expenses Database'!D125</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B126" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" s="20">
+        <f>+'Actuals Expenses Database'!D126-'Forecast Expenses Database'!D126</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B127" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C127" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="20">
+        <f>+'Actuals Expenses Database'!D127-'Forecast Expenses Database'!D127</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B128" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D128" s="20">
+        <f>+'Actuals Expenses Database'!D128-'Forecast Expenses Database'!D128</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B129" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C129" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" s="20">
+        <f>+'Actuals Expenses Database'!D129-'Forecast Expenses Database'!D129</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B130" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="20">
+        <f>+'Actuals Expenses Database'!D130-'Forecast Expenses Database'!D130</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B131" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" s="20">
+        <f>+'Actuals Expenses Database'!D131-'Forecast Expenses Database'!D131</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B132" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C132" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" s="20">
+        <f>+'Actuals Expenses Database'!D132-'Forecast Expenses Database'!D132</f>
+        <v>-73.623600565533707</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133" s="20">
+        <f>+'Actuals Expenses Database'!D133-'Forecast Expenses Database'!D133</f>
+        <v>-151.12588826594259</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B134" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" s="20">
+        <f>+'Actuals Expenses Database'!D134-'Forecast Expenses Database'!D134</f>
+        <v>144.165831443868</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B135" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="20">
+        <f>+'Actuals Expenses Database'!D135-'Forecast Expenses Database'!D135</f>
+        <v>158.74436326821183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B136" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" s="20">
+        <f>+'Actuals Expenses Database'!D136-'Forecast Expenses Database'!D136</f>
+        <v>-10.782902159329979</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B137" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137" s="20">
+        <f>+'Actuals Expenses Database'!D137-'Forecast Expenses Database'!D137</f>
+        <v>133.71863041374729</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B138" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" s="20">
+        <f>+'Actuals Expenses Database'!D138-'Forecast Expenses Database'!D138</f>
+        <v>129.46241887343592</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B139" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" s="20">
+        <f>+'Actuals Expenses Database'!D139-'Forecast Expenses Database'!D139</f>
+        <v>66.71146607371179</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B140" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" s="20">
+        <f>+'Actuals Expenses Database'!D140-'Forecast Expenses Database'!D140</f>
+        <v>135.67306071726398</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B141" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C141" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" s="20">
+        <f>+'Actuals Expenses Database'!D141-'Forecast Expenses Database'!D141</f>
+        <v>51.340366289342455</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B142" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C142" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142" s="20">
+        <f>+'Actuals Expenses Database'!D142-'Forecast Expenses Database'!D142</f>
+        <v>100.30651576774267</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B143" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="20">
+        <f>+'Actuals Expenses Database'!D143-'Forecast Expenses Database'!D143</f>
+        <v>242.12127357705424</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B144" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C144" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" s="20">
+        <f>+'Actuals Expenses Database'!D144-'Forecast Expenses Database'!D144</f>
+        <v>926.71153543357104</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B145" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="20">
+        <f>+'Actuals Expenses Database'!D145-'Forecast Expenses Database'!D145</f>
+        <v>185.76307609835567</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B146" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D146" s="20">
+        <f>+'Actuals Expenses Database'!D146-'Forecast Expenses Database'!D146</f>
+        <v>-69.234064013659008</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B147" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" s="20">
+        <f>+'Actuals Expenses Database'!D147-'Forecast Expenses Database'!D147</f>
+        <v>497.74192309137834</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B148" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D148" s="20">
+        <f>+'Actuals Expenses Database'!D148-'Forecast Expenses Database'!D148</f>
+        <v>-188.81275764642305</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B149" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D149" s="20">
+        <f>+'Actuals Expenses Database'!D149-'Forecast Expenses Database'!D149</f>
+        <v>-156.50739269233782</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B150" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="20">
+        <f>+'Actuals Expenses Database'!D150-'Forecast Expenses Database'!D150</f>
+        <v>2.4224695678349235</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B151" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C151" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" s="20">
+        <f>+'Actuals Expenses Database'!D151-'Forecast Expenses Database'!D151</f>
+        <v>191.04907367895066</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B152" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C152" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="20">
+        <f>+'Actuals Expenses Database'!D152-'Forecast Expenses Database'!D152</f>
+        <v>-22.560978022009294</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B153" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C153" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" s="20">
+        <f>+'Actuals Expenses Database'!D153-'Forecast Expenses Database'!D153</f>
+        <v>184.27010771492132</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B154" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C154" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D154" s="20">
+        <f>+'Actuals Expenses Database'!D154-'Forecast Expenses Database'!D154</f>
+        <v>235.50221111417704</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B155" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C155" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D155" s="20">
+        <f>+'Actuals Expenses Database'!D155-'Forecast Expenses Database'!D155</f>
+        <v>169.26193683985184</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B156" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="20">
+        <f>+'Actuals Expenses Database'!D156-'Forecast Expenses Database'!D156</f>
+        <v>580.48450649080951</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B157" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C157" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" s="20">
+        <f>+'Actuals Expenses Database'!D157-'Forecast Expenses Database'!D157</f>
+        <v>1609.380112221872</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B158" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="20">
+        <f>+'Actuals Expenses Database'!D158-'Forecast Expenses Database'!D158</f>
+        <v>314.75840024750596</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B159" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C159" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D159" s="20">
+        <f>+'Actuals Expenses Database'!D159-'Forecast Expenses Database'!D159</f>
+        <v>-365.87596236208037</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B160" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C160" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" s="20">
+        <f>+'Actuals Expenses Database'!D160-'Forecast Expenses Database'!D160</f>
+        <v>-60.003416630986749</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B161" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C161" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D161" s="20">
+        <f>+'Actuals Expenses Database'!D161-'Forecast Expenses Database'!D161</f>
+        <v>-212.29315965136811</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B162" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C162" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D162" s="20">
+        <f>+'Actuals Expenses Database'!D162-'Forecast Expenses Database'!D162</f>
+        <v>81.385892323389271</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B163" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C163" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D163" s="20">
+        <f>+'Actuals Expenses Database'!D163-'Forecast Expenses Database'!D163</f>
+        <v>62.602502454999467</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B164" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C164" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" s="20">
+        <f>+'Actuals Expenses Database'!D164-'Forecast Expenses Database'!D164</f>
+        <v>64.795504401993639</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B165" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="20">
+        <f>+'Actuals Expenses Database'!D165-'Forecast Expenses Database'!D165</f>
+        <v>288.70188730887821</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B166" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C166" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D166" s="20">
+        <f>+'Actuals Expenses Database'!D166-'Forecast Expenses Database'!D166</f>
+        <v>-210.87745580768024</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B167" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C167" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D167" s="20">
+        <f>+'Actuals Expenses Database'!D167-'Forecast Expenses Database'!D167</f>
+        <v>-364.0768277206962</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B168" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C168" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D168" s="20">
+        <f>+'Actuals Expenses Database'!D168-'Forecast Expenses Database'!D168</f>
+        <v>-88.853891985593691</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B169" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C169" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" s="20">
+        <f>+'Actuals Expenses Database'!D169-'Forecast Expenses Database'!D169</f>
+        <v>-17.719739893254655</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B170" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C170" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D170" s="20">
+        <f>+'Actuals Expenses Database'!D170-'Forecast Expenses Database'!D170</f>
+        <v>-507.45626731489028</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B171" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="20">
+        <f>+'Actuals Expenses Database'!D171-'Forecast Expenses Database'!D171</f>
+        <v>-1526.3917319029772</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B172" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C172" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D172" s="20">
+        <f>+'Actuals Expenses Database'!D172-'Forecast Expenses Database'!D172</f>
+        <v>-1696.4426915331601</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B173" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C173" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="20">
+        <f>+'Actuals Expenses Database'!D173-'Forecast Expenses Database'!D173</f>
+        <v>-2073.0580475273246</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B174" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D174" s="20">
+        <f>+'Actuals Expenses Database'!D174-'Forecast Expenses Database'!D174</f>
+        <v>-2300.0695894314508</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B175" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C175" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="20">
+        <f>+'Actuals Expenses Database'!D175-'Forecast Expenses Database'!D175</f>
+        <v>-1862.2670439400988</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B176" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C176" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" s="20">
+        <f>+'Actuals Expenses Database'!D176-'Forecast Expenses Database'!D176</f>
+        <v>-2113.9546131729185</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B177" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C177" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" s="20">
+        <f>+'Actuals Expenses Database'!D177-'Forecast Expenses Database'!D177</f>
+        <v>-2330.202220091764</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B178" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C178" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="20">
+        <f>+'Actuals Expenses Database'!D178-'Forecast Expenses Database'!D178</f>
+        <v>-1921.7591861921649</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B179" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C179" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D179" s="20">
+        <f>+'Actuals Expenses Database'!D179-'Forecast Expenses Database'!D179</f>
+        <v>-1808.8964708527469</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B180" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D180" s="20">
+        <f>+'Actuals Expenses Database'!D180-'Forecast Expenses Database'!D180</f>
+        <v>-2176.3532222074268</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B181" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C181" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" s="20">
+        <f>+'Actuals Expenses Database'!D181-'Forecast Expenses Database'!D181</f>
+        <v>-2174.4585625461264</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B182" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" s="20">
+        <f>+'Actuals Expenses Database'!D182-'Forecast Expenses Database'!D182</f>
+        <v>-1988.8055936837791</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B183" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C183" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D183" s="20">
+        <f>+'Actuals Expenses Database'!D183-'Forecast Expenses Database'!D183</f>
+        <v>-23972.65897308194</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B184" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" s="20">
+        <f>+'Actuals Expenses Database'!D184-'Forecast Expenses Database'!D184</f>
+        <v>-1211.6333316554715</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B185" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D185" s="20">
+        <f>+'Actuals Expenses Database'!D185-'Forecast Expenses Database'!D185</f>
+        <v>-2062.3186538952405</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B186" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C186" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D186" s="20">
+        <f>+'Actuals Expenses Database'!D186-'Forecast Expenses Database'!D186</f>
+        <v>-2133.0614641583115</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B187" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D187" s="20">
+        <f>+'Actuals Expenses Database'!D187-'Forecast Expenses Database'!D187</f>
+        <v>-2512.3627490828189</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B188" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D188" s="20">
+        <f>+'Actuals Expenses Database'!D188-'Forecast Expenses Database'!D188</f>
+        <v>-1780.8811516167093</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B189" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D189" s="20">
+        <f>+'Actuals Expenses Database'!D189-'Forecast Expenses Database'!D189</f>
+        <v>-2051.352110717919</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B190" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C190" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D190" s="20">
+        <f>+'Actuals Expenses Database'!D190-'Forecast Expenses Database'!D190</f>
+        <v>-2265.4067156897704</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B191" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" s="20">
+        <f>+'Actuals Expenses Database'!D191-'Forecast Expenses Database'!D191</f>
+        <v>-1633.0572988832869</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B192" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C192" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="20">
+        <f>+'Actuals Expenses Database'!D192-'Forecast Expenses Database'!D192</f>
+        <v>-2019.7739266604272</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B193" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C193" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" s="20">
+        <f>+'Actuals Expenses Database'!D193-'Forecast Expenses Database'!D193</f>
+        <v>-2540.4300499281226</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B194" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D194" s="20">
+        <f>+'Actuals Expenses Database'!D194-'Forecast Expenses Database'!D194</f>
+        <v>-2263.3124545317196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B195" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="20">
+        <f>+'Actuals Expenses Database'!D195-'Forecast Expenses Database'!D195</f>
+        <v>-2006.5253335770337</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B196" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="20">
+        <f>+'Actuals Expenses Database'!D196-'Forecast Expenses Database'!D196</f>
+        <v>-24480.11524039683</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B197" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D197" s="20">
+        <f>+'Actuals Expenses Database'!D197-'Forecast Expenses Database'!D197</f>
+        <v>-1662.3787883076293</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B198" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C198" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D198" s="20">
+        <f>+'Actuals Expenses Database'!D198-'Forecast Expenses Database'!D198</f>
+        <v>-1998.3396441996447</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B199" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C199" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D199" s="20">
+        <f>+'Actuals Expenses Database'!D199-'Forecast Expenses Database'!D199</f>
+        <v>-1470.2450831298192</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B200" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C200" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D200" s="20">
+        <f>+'Actuals Expenses Database'!D200-'Forecast Expenses Database'!D200</f>
+        <v>-2651.5210943295242</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B201" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C201" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D201" s="20">
+        <f>+'Actuals Expenses Database'!D201-'Forecast Expenses Database'!D201</f>
+        <v>-2286.3921678923507</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B202" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C202" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D202" s="20">
+        <f>+'Actuals Expenses Database'!D202-'Forecast Expenses Database'!D202</f>
+        <v>-2438.6635718157486</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B203" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C203" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="20">
+        <f>+'Actuals Expenses Database'!D203-'Forecast Expenses Database'!D203</f>
+        <v>-2194.6402780733042</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B204" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C204" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" s="20">
+        <f>+'Actuals Expenses Database'!D204-'Forecast Expenses Database'!D204</f>
+        <v>-1658.936857820896</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B205" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C205" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D205" s="20">
+        <f>+'Actuals Expenses Database'!D205-'Forecast Expenses Database'!D205</f>
+        <v>-1401.3260073322162</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B206" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C206" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D206" s="20">
+        <f>+'Actuals Expenses Database'!D206-'Forecast Expenses Database'!D206</f>
+        <v>-2297.6496555925696</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B207" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C207" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D207" s="20">
+        <f>+'Actuals Expenses Database'!D207-'Forecast Expenses Database'!D207</f>
+        <v>-2187.618468256609</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B208" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C208" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D208" s="20">
+        <f>+'Actuals Expenses Database'!D208-'Forecast Expenses Database'!D208</f>
+        <v>-1341.4716688564222</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B209" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D209" s="20">
+        <f>+'Actuals Expenses Database'!D209-'Forecast Expenses Database'!D209</f>
+        <v>-23589.183285606792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor theme="4"/>
@@ -20086,7 +23240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="7" tint="-0.499984740745262"/>
@@ -20094,7 +23248,7 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -22003,7 +25157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="4" tint="0.79998168889431442"/>

</xml_diff>